<commit_message>
Updated default browser to Chrome
</commit_message>
<xml_diff>
--- a/src/test/java/dataEngine/Asset Feature Deletion.xlsx
+++ b/src/test/java/dataEngine/Asset Feature Deletion.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="30" windowWidth="18195" windowHeight="10290"/>
@@ -51,9 +51,6 @@
     <t>openBrowser</t>
   </si>
   <si>
-    <t>Mozilla</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>maxadmin</t>
+  </si>
+  <si>
+    <t>Chrome</t>
   </si>
 </sst>
 </file>
@@ -206,8 +206,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -506,7 +534,7 @@
   <dimension ref="A1:L140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,10 +581,10 @@
     </row>
     <row r="2" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="15" t="s">
@@ -570,7 +598,7 @@
         <v>10</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="12"/>
@@ -579,70 +607,70 @@
     </row>
     <row r="3" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3" s="14"/>
       <c r="J3" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="18" t="s">
         <v>14</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>15</v>
       </c>
       <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="18">
         <v>1</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" s="18">
         <v>1</v>

</xml_diff>